<commit_message>
crane edits and simple blade transport model as advised by industry
</commit_message>
<xml_diff>
--- a/project_input_template/project_data/ge15_expected_validation.xlsx
+++ b/project_input_template/project_data/ge15_expected_validation.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akey/Projects/WISDEM/WISDEM/wisdem/library/landbosse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/WISDEM/wisdem/library/landbosse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8906BF94-CBF0-EC41-8429-218A21ABCD49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FA9311-4BC4-834F-93DA-047E194A2EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20880" yWindow="460" windowWidth="28720" windowHeight="23320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9700" yWindow="500" windowWidth="28720" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costs_by_module_type_operation" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">costs_by_module_type_operation!$A$1:$G$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">costs_by_module_type_operation!$A$1:$G$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="39">
   <si>
     <t>FoundationCost</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>WISDEM</t>
+  </si>
+  <si>
+    <t>TransportCost</t>
+  </si>
+  <si>
+    <t>Transport</t>
   </si>
 </sst>
 </file>
@@ -220,9 +226,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -260,9 +266,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -295,26 +301,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -347,26 +336,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -540,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -832,16 +804,16 @@
         <v>1.5</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
       </c>
       <c r="G12">
-        <v>4084775.1528987698</v>
+        <v>1190000</v>
       </c>
       <c r="H12"/>
     </row>
@@ -856,16 +828,16 @@
         <v>1.5</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G13">
-        <v>426614.68629607599</v>
+        <v>4084775.1528987698</v>
       </c>
       <c r="H13"/>
     </row>
@@ -886,10 +858,10 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14">
-        <v>1402888.02678423</v>
+        <v>426614.68629607599</v>
       </c>
       <c r="H14"/>
     </row>
@@ -910,10 +882,10 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15">
-        <v>2808055.1406992902</v>
+        <v>1402888.02678423</v>
       </c>
       <c r="H15"/>
     </row>
@@ -934,10 +906,10 @@
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G16">
-        <v>231877.89268898001</v>
+        <v>2808055.1406992902</v>
       </c>
       <c r="H16"/>
     </row>
@@ -952,16 +924,16 @@
         <v>1.5</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>231877.89268898001</v>
       </c>
       <c r="H17"/>
     </row>
@@ -982,10 +954,10 @@
         <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="H18"/>
     </row>
@@ -1006,10 +978,10 @@
         <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="H19"/>
     </row>
@@ -1030,7 +1002,7 @@
         <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1054,7 +1026,7 @@
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1072,16 +1044,16 @@
         <v>1.5</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G22">
-        <v>730892.72216529795</v>
+        <v>0</v>
       </c>
       <c r="H22"/>
     </row>
@@ -1102,10 +1074,10 @@
         <v>13</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G23">
-        <v>28266</v>
+        <v>730892.72216529795</v>
       </c>
       <c r="H23"/>
     </row>
@@ -1126,10 +1098,10 @@
         <v>13</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G24">
-        <v>5076630.5559791401</v>
+        <v>28266</v>
       </c>
       <c r="H24"/>
     </row>
@@ -1150,10 +1122,10 @@
         <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G25">
-        <v>899310</v>
+        <v>5076630.5559791401</v>
       </c>
       <c r="H25"/>
     </row>
@@ -1174,10 +1146,10 @@
         <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>899310</v>
       </c>
       <c r="H26"/>
     </row>
@@ -1198,7 +1170,7 @@
         <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1216,16 +1188,16 @@
         <v>1.5</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G28">
-        <v>191287.126780697</v>
+        <v>0</v>
       </c>
       <c r="H28"/>
     </row>
@@ -1246,10 +1218,10 @@
         <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G29">
-        <v>395666.692613583</v>
+        <v>197951.126780675</v>
       </c>
       <c r="H29"/>
     </row>
@@ -1270,10 +1242,10 @@
         <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G30">
-        <v>1884677.4314043</v>
+        <v>395666.692613583</v>
       </c>
       <c r="H30"/>
     </row>
@@ -1294,10 +1266,10 @@
         <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G31">
-        <v>341584.15496552998</v>
+        <v>1884677.4314043</v>
       </c>
       <c r="H31"/>
     </row>
@@ -1318,10 +1290,10 @@
         <v>14</v>
       </c>
       <c r="F32" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G32">
-        <v>4447425.6976512</v>
+        <v>353484.15496549098</v>
       </c>
       <c r="H32"/>
     </row>
@@ -1342,10 +1314,10 @@
         <v>14</v>
       </c>
       <c r="F33" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G33">
-        <v>2071325</v>
+        <v>4602363.6976506999</v>
       </c>
       <c r="H33"/>
     </row>
@@ -1366,15 +1338,39 @@
         <v>14</v>
       </c>
       <c r="F34" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34">
+        <v>2071325</v>
+      </c>
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>100</v>
+      </c>
+      <c r="C35">
+        <v>1.5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" t="s">
         <v>27</v>
       </c>
-      <c r="G34">
+      <c r="G35">
         <v>1306167.9333333301</v>
       </c>
-      <c r="H34"/>
+      <c r="H35"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G34" xr:uid="{74B3986E-2BCE-704E-B480-617FD308BB93}"/>
+  <autoFilter ref="A1:G35" xr:uid="{74B3986E-2BCE-704E-B480-617FD308BB93}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
passing all tests locally
</commit_message>
<xml_diff>
--- a/project_input_template/project_data/ge15_expected_validation.xlsx
+++ b/project_input_template/project_data/ge15_expected_validation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/WISDEM/wisdem/library/landbosse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/LandBOSSE/project_input_template/project_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FA9311-4BC4-834F-93DA-047E194A2EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10402C75-5DF7-4143-9078-3EB5EC72F809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9700" yWindow="500" windowWidth="28720" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9680" yWindow="500" windowWidth="28720" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costs_by_module_type_operation" sheetId="1" r:id="rId1"/>
@@ -515,7 +515,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G29" sqref="G29:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -813,7 +813,7 @@
         <v>19</v>
       </c>
       <c r="G12">
-        <v>1190000</v>
+        <v>12320000</v>
       </c>
       <c r="H12"/>
     </row>
@@ -1221,7 +1221,7 @@
         <v>24</v>
       </c>
       <c r="G29">
-        <v>197951.126780675</v>
+        <v>260279.126780675</v>
       </c>
       <c r="H29"/>
     </row>
@@ -1245,7 +1245,7 @@
         <v>22</v>
       </c>
       <c r="G30">
-        <v>395666.692613583</v>
+        <v>395666.69261350599</v>
       </c>
       <c r="H30"/>
     </row>
@@ -1293,7 +1293,7 @@
         <v>21</v>
       </c>
       <c r="G32">
-        <v>353484.15496549098</v>
+        <v>464784.15496549098</v>
       </c>
       <c r="H32"/>
     </row>
@@ -1317,7 +1317,7 @@
         <v>25</v>
       </c>
       <c r="G33">
-        <v>4602363.6976506999</v>
+        <v>6051489.6976506999</v>
       </c>
       <c r="H33"/>
     </row>

</xml_diff>

<commit_message>
update test expected result
</commit_message>
<xml_diff>
--- a/project_input_template/project_data/ge15_expected_validation.xlsx
+++ b/project_input_template/project_data/ge15_expected_validation.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/LandBOSSE/project_input_template/project_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcrook\nrel\github\LandBOSSE\input\project_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10402C75-5DF7-4143-9078-3EB5EC72F809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B79682-D817-49EC-8218-147192497AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9680" yWindow="500" windowWidth="28720" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costs_by_module_type_operation" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">costs_by_module_type_operation!$A$1:$G$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">costs_by_module_type_operation!$A$1:$G$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="41">
   <si>
     <t>FoundationCost</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Number of turbines</t>
   </si>
   <si>
-    <t>Turbine rating MW</t>
-  </si>
-  <si>
     <t>Project ID with serial</t>
   </si>
   <si>
@@ -150,6 +147,15 @@
   </si>
   <si>
     <t>Transport</t>
+  </si>
+  <si>
+    <t>Turbine rating (MW)</t>
+  </si>
+  <si>
+    <t>TurbineCost</t>
+  </si>
+  <si>
+    <t>Turbine</t>
   </si>
 </sst>
 </file>
@@ -512,50 +518,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29:G33"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -573,13 +577,13 @@
         <v>15</v>
       </c>
       <c r="G2">
-        <v>299607.30011378299</v>
+        <v>299607.30011378002</v>
       </c>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -597,13 +601,13 @@
         <v>16</v>
       </c>
       <c r="G3">
-        <v>3593613.2013053899</v>
+        <v>3593613.2013053601</v>
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -621,13 +625,13 @@
         <v>17</v>
       </c>
       <c r="G4">
-        <v>5424241.0516086202</v>
+        <v>5424241.0516085699</v>
       </c>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -645,13 +649,12 @@
         <v>18</v>
       </c>
       <c r="G5">
-        <v>465873.07765138999</v>
-      </c>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>465873.07765138499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -671,11 +674,10 @@
       <c r="G6">
         <v>797751.53459731699</v>
       </c>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -695,11 +697,10 @@
       <c r="G7">
         <v>412013.84003877599</v>
       </c>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>100</v>
@@ -719,11 +720,10 @@
       <c r="G8">
         <v>609463.12967557705</v>
       </c>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -743,11 +743,10 @@
       <c r="G9">
         <v>1307300.76</v>
       </c>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>100</v>
@@ -767,11 +766,10 @@
       <c r="G10">
         <v>83009.351967474897</v>
       </c>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11">
         <v>100</v>
@@ -791,23 +789,22 @@
       <c r="G11">
         <v>4859182.0720829004</v>
       </c>
-      <c r="H11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>1.5</v>
+      </c>
+      <c r="D12" t="s">
         <v>36</v>
       </c>
-      <c r="B12">
-        <v>100</v>
-      </c>
-      <c r="C12">
-        <v>1.5</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>37</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -815,11 +812,10 @@
       <c r="G12">
         <v>12320000</v>
       </c>
-      <c r="H12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -831,7 +827,7 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" t="s">
         <v>19</v>
@@ -839,11 +835,10 @@
       <c r="G13">
         <v>4084775.1528987698</v>
       </c>
-      <c r="H13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14">
         <v>100</v>
@@ -861,13 +856,12 @@
         <v>15</v>
       </c>
       <c r="G14">
-        <v>426614.68629607599</v>
-      </c>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>497045.44340216101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>100</v>
@@ -885,13 +879,12 @@
         <v>16</v>
       </c>
       <c r="G15">
-        <v>1402888.02678423</v>
-      </c>
-      <c r="H15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1560537.3987719801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>100</v>
@@ -909,13 +902,12 @@
         <v>17</v>
       </c>
       <c r="G16">
-        <v>2808055.1406992902</v>
-      </c>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>3334332.4600047702</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17">
         <v>100</v>
@@ -933,13 +925,12 @@
         <v>18</v>
       </c>
       <c r="G17">
-        <v>231877.89268898001</v>
-      </c>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>269595.76510894601</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>100</v>
@@ -959,11 +950,10 @@
       <c r="G18">
         <v>0</v>
       </c>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19">
         <v>100</v>
@@ -983,11 +973,10 @@
       <c r="G19">
         <v>1000000</v>
       </c>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20">
         <v>100</v>
@@ -1007,11 +996,10 @@
       <c r="G20">
         <v>0</v>
       </c>
-      <c r="H20"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21">
         <v>100</v>
@@ -1031,11 +1019,10 @@
       <c r="G21">
         <v>0</v>
       </c>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22">
         <v>100</v>
@@ -1055,11 +1042,10 @@
       <c r="G22">
         <v>0</v>
       </c>
-      <c r="H22"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>100</v>
@@ -1068,22 +1054,21 @@
         <v>1.5</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G23">
-        <v>730892.72216529795</v>
-      </c>
-      <c r="H23"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24">
         <v>100</v>
@@ -1098,16 +1083,15 @@
         <v>13</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G24">
-        <v>28266</v>
-      </c>
-      <c r="H24"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>570674.28623627801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25">
         <v>100</v>
@@ -1122,16 +1106,15 @@
         <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G25">
-        <v>5076630.5559791401</v>
-      </c>
-      <c r="H25"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23472</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26">
         <v>100</v>
@@ -1146,16 +1129,15 @@
         <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G26">
-        <v>899310</v>
-      </c>
-      <c r="H26"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>4558948.42278203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>100</v>
@@ -1170,16 +1152,15 @@
         <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1213156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28">
         <v>100</v>
@@ -1194,16 +1175,15 @@
         <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
-      <c r="H28"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29">
         <v>100</v>
@@ -1212,22 +1192,21 @@
         <v>1.5</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G29">
-        <v>260279.126780675</v>
-      </c>
-      <c r="H29"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>100</v>
@@ -1242,16 +1221,15 @@
         <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G30">
-        <v>395666.69261350599</v>
-      </c>
-      <c r="H30"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>262649.19659017801</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31">
         <v>100</v>
@@ -1266,16 +1244,15 @@
         <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G31">
-        <v>1884677.4314043</v>
-      </c>
-      <c r="H31"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>395666.69261358201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>100</v>
@@ -1290,16 +1267,15 @@
         <v>14</v>
       </c>
       <c r="F32" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G32">
-        <v>464784.15496549098</v>
-      </c>
-      <c r="H32"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1820552.416185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>100</v>
@@ -1314,16 +1290,15 @@
         <v>14</v>
       </c>
       <c r="F33" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G33">
-        <v>6051489.6976506999</v>
-      </c>
-      <c r="H33"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>469016.42248246103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>100</v>
@@ -1338,16 +1313,15 @@
         <v>14</v>
       </c>
       <c r="F34" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G34">
-        <v>2071325</v>
-      </c>
-      <c r="H34"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>6106593.8207216403</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35">
         <v>100</v>
@@ -1362,15 +1336,37 @@
         <v>14</v>
       </c>
       <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35">
+        <v>2071325</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>100</v>
+      </c>
+      <c r="C36">
+        <v>1.5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" t="s">
         <v>27</v>
       </c>
-      <c r="G35">
-        <v>1306167.9333333301</v>
-      </c>
-      <c r="H35"/>
+      <c r="G36">
+        <v>1294172.6187036999</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G35" xr:uid="{74B3986E-2BCE-704E-B480-617FD308BB93}"/>
+  <autoFilter ref="A1:G4" xr:uid="{74B3986E-2BCE-704E-B480-617FD308BB93}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>